<commit_message>
added internal gains in heating shifting, revised units of measure in launcher_shift2
</commit_message>
<xml_diff>
--- a/test4f.xlsx
+++ b/test4f.xlsx
@@ -1851,13 +1851,13 @@
       <c r="S13" t="inlineStr"/>
       <c r="T13" t="inlineStr"/>
       <c r="U13" t="n">
-        <v>9.232996483297564</v>
+        <v>10</v>
       </c>
       <c r="V13" t="n">
         <v>0</v>
       </c>
       <c r="W13" t="n">
-        <v>13849.49472494635</v>
+        <v>15000</v>
       </c>
       <c r="X13" t="n">
         <v>0</v>
@@ -1871,77 +1871,77 @@
       <c r="AE13" t="inlineStr"/>
       <c r="AF13" t="inlineStr"/>
       <c r="AG13" t="n">
-        <v>8.159029476741042</v>
+        <v>7.727832487873169</v>
       </c>
       <c r="AH13" t="n">
-        <v>13554.68766721154</v>
+        <v>11559.42574525542</v>
       </c>
       <c r="AI13" t="n">
-        <v>9755.919730798634</v>
+        <v>10566.36352937754</v>
       </c>
       <c r="AJ13" t="n">
-        <v>2973.569625384749</v>
+        <v>3521.330594287391</v>
       </c>
       <c r="AK13" t="n">
-        <v>6782.350105413922</v>
+        <v>7045.032935090147</v>
       </c>
       <c r="AL13" t="n">
-        <v>10581.11804182718</v>
+        <v>8038.095150968032</v>
       </c>
       <c r="AM13" t="n">
-        <v>2650.390947447119</v>
+        <v>607.1753285511822</v>
       </c>
       <c r="AN13" t="n">
-        <v>2028.134578222797</v>
+        <v>1482.44036143576</v>
       </c>
       <c r="AO13" t="n">
-        <v>4053.348816503142</v>
+        <v>4116.063933945034</v>
       </c>
       <c r="AP13" t="n">
-        <v>1849.243699653907</v>
+        <v>1832.415527036056</v>
       </c>
       <c r="AQ13" t="n">
-        <v>14.92666685128674</v>
+        <v>-0.6345958244451267</v>
       </c>
       <c r="AR13" t="n">
-        <v>3.0734468400506</v>
+        <v>-8.42685369907935</v>
       </c>
       <c r="AS13" t="n">
-        <v>-6.589719684481667</v>
+        <v>-21.29685747924691</v>
       </c>
       <c r="AT13" t="n">
-        <v>1.941233320360956</v>
+        <v>-0.1045435911062923</v>
       </c>
       <c r="AU13" t="n">
-        <v>0.2193757391088945</v>
+        <v>0.3046285059387767</v>
       </c>
       <c r="AV13" t="n">
-        <v>0.3047964423074777</v>
+        <v>0.3332585126848113</v>
       </c>
       <c r="AW13" t="n">
         <v>0</v>
       </c>
       <c r="AX13" t="n">
-        <v>271.2940042165569</v>
+        <v>281.8013174036062</v>
       </c>
       <c r="AY13" t="n">
-        <v>2829.440759434487</v>
+        <v>2286.96504063424</v>
       </c>
       <c r="AZ13" t="n">
         <v>0</v>
       </c>
       <c r="BA13" t="n">
-        <v>-2558.14675521793</v>
+        <v>-2005.163723230634</v>
       </c>
       <c r="BB13" t="n">
-        <v>0.2860418889241081</v>
+        <v>0.2970564980271703</v>
       </c>
       <c r="BC13" t="inlineStr"/>
       <c r="BD13" t="n">
-        <v>-17392.90727233772</v>
+        <v>-2185.954915917501</v>
       </c>
       <c r="BE13" t="n">
-        <v>-1.25585139514215</v>
+        <v>-0.1457303277278334</v>
       </c>
     </row>
     <row r="14">

</xml_diff>

<commit_message>
solved issue on shifting house heating
</commit_message>
<xml_diff>
--- a/test4f.xlsx
+++ b/test4f.xlsx
@@ -1871,77 +1871,77 @@
       <c r="AE13" t="inlineStr"/>
       <c r="AF13" t="inlineStr"/>
       <c r="AG13" t="n">
-        <v>7.727832487873169</v>
+        <v>9.14482161880739</v>
       </c>
       <c r="AH13" t="n">
-        <v>11559.42574525542</v>
+        <v>15825.33339008426</v>
       </c>
       <c r="AI13" t="n">
-        <v>10566.36352937754</v>
+        <v>10476</v>
       </c>
       <c r="AJ13" t="n">
-        <v>3521.330594287391</v>
+        <v>3471.728204622751</v>
       </c>
       <c r="AK13" t="n">
-        <v>7045.032935090147</v>
+        <v>7004.271795377251</v>
       </c>
       <c r="AL13" t="n">
-        <v>8038.095150968032</v>
+        <v>12353.60518546151</v>
       </c>
       <c r="AM13" t="n">
-        <v>607.1753285511822</v>
+        <v>2994.013868898331</v>
       </c>
       <c r="AN13" t="n">
-        <v>1482.44036143576</v>
+        <v>2445.786307273602</v>
       </c>
       <c r="AO13" t="n">
-        <v>4116.063933945034</v>
+        <v>4814.27754107044</v>
       </c>
       <c r="AP13" t="n">
-        <v>1832.415527036056</v>
+        <v>2099.527468219139</v>
       </c>
       <c r="AQ13" t="n">
-        <v>-0.6345958244451267</v>
+        <v>-0.6740005041031701</v>
       </c>
       <c r="AR13" t="n">
-        <v>-8.42685369907935</v>
+        <v>-6.437845823738465</v>
       </c>
       <c r="AS13" t="n">
-        <v>-21.29685747924691</v>
+        <v>-14.73959102415433</v>
       </c>
       <c r="AT13" t="n">
-        <v>-0.1045435911062923</v>
+        <v>-0.08635137603200758</v>
       </c>
       <c r="AU13" t="n">
-        <v>0.3046285059387767</v>
+        <v>0.2193778872802796</v>
       </c>
       <c r="AV13" t="n">
-        <v>0.3332585126848113</v>
+        <v>0.331398263136956</v>
       </c>
       <c r="AW13" t="n">
         <v>0</v>
       </c>
       <c r="AX13" t="n">
-        <v>281.8013174036062</v>
+        <v>280.1708718150903</v>
       </c>
       <c r="AY13" t="n">
-        <v>2286.96504063424</v>
+        <v>3306.052148343698</v>
       </c>
       <c r="AZ13" t="n">
         <v>0</v>
       </c>
       <c r="BA13" t="n">
-        <v>-2005.163723230634</v>
+        <v>-3025.881276528608</v>
       </c>
       <c r="BB13" t="n">
-        <v>0.2970564980271703</v>
+        <v>0.2814803312251295</v>
       </c>
       <c r="BC13" t="inlineStr"/>
       <c r="BD13" t="n">
-        <v>-2185.954915917501</v>
+        <v>-2441.954144085222</v>
       </c>
       <c r="BE13" t="n">
-        <v>-0.1457303277278334</v>
+        <v>-0.1627969429390148</v>
       </c>
     </row>
     <row r="14">

</xml_diff>